<commit_message>
Se agrego el primer prototipo de hacer reservas en usuarios
</commit_message>
<xml_diff>
--- a/Proyecto1/bin/Debug/Entrenadores.xlsx
+++ b/Proyecto1/bin/Debug/Entrenadores.xlsx
@@ -56,61 +56,61 @@
     <x:t>Argba</x:t>
   </x:si>
   <x:si>
+    <x:t>CardioDance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bonnie639</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P35ñ08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bonnie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Emeron</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ada1179</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P35ñ09</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ada</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wong</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Funcionales</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gabriel7794</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P35ñ10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gabriel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mazariegos</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yalin1110</x:t>
+  </x:si>
+  <x:si>
+    <x:t>P35ñ11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yalin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Campos</x:t>
+  </x:si>
+  <x:si>
     <x:t>Zumba</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bonnie639</x:t>
-  </x:si>
-  <x:si>
-    <x:t>P35ñ08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bonnie</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Emeron</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CardioDance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ada1179</x:t>
-  </x:si>
-  <x:si>
-    <x:t>P35ñ09</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ada</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Wong</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Funcionales</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gabriel7794</x:t>
-  </x:si>
-  <x:si>
-    <x:t>P35ñ10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gabriel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mazariegos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Yalin1110</x:t>
-  </x:si>
-  <x:si>
-    <x:t>P35ñ11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Yalin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Campos</x:t>
   </x:si>
   <x:si>
     <x:t>German15</x:t>
@@ -635,70 +635,70 @@
         <x:v>1237895</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G3" s="7"/>
     </x:row>
     <x:row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <x:c r="A4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="C4" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>20</x:v>
       </x:c>
       <x:c r="E4" s="0">
         <x:v>1237896</x:v>
       </x:c>
       <x:c r="F4" s="6" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G4" s="7"/>
     </x:row>
     <x:row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <x:c r="A5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
+      <x:c r="D5" s="0" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>25</x:v>
       </x:c>
       <x:c r="E5" s="0">
         <x:v>1237897</x:v>
       </x:c>
       <x:c r="F5" s="6" t="s">
-        <x:v>21</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G5" s="7"/>
     </x:row>
     <x:row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <x:c r="A6" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
+      <x:c r="C6" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="D6" s="0" t="s">
         <x:v>28</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
       <x:c r="E6" s="0">
         <x:v>1237898</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G6" s="7"/>
     </x:row>
@@ -719,7 +719,7 @@
         <x:v>1237899</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G7" s="7"/>
     </x:row>

</xml_diff>